<commit_message>
update Michele 2 sept 2019
</commit_message>
<xml_diff>
--- a/simmod/partitioning/wofost from Raul/Partitioning_WOFOST.xlsx
+++ b/simmod/partitioning/wofost from Raul/Partitioning_WOFOST.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\meronmi\Documents\IDL\simmod\partitioning\wofost from Raul\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\IDL\simmod\partitioning\wofost from Raul\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="11805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>leaves</t>
   </si>
@@ -74,7 +74,10 @@
     <t>Leaves over total</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Leaves over total correct</t>
+  </si>
+  <si>
+    <t>il nostro start non e' DVS = 0</t>
   </si>
 </sst>
 </file>
@@ -884,24 +887,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$12</c:f>
+              <c:f>Sheet1!$L$5:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.32500000000000001</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32500000000000001</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27999999999999997</c:v>
+                  <c:v>0.24899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1000000000000004E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -910,12 +913,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3628,10 +3625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3644,7 +3641,7 @@
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
@@ -3657,7 +3654,7 @@
       <c r="G1" s="15"/>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
@@ -3686,7 +3683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -3716,8 +3713,12 @@
         <f>F3*C3</f>
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f>D3*F3</f>
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="9">
         <v>0.1</v>
@@ -3745,8 +3746,12 @@
         <f t="shared" ref="J4:J22" si="1">F4*C4</f>
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" ref="L4:L12" si="2">D4*F4</f>
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="9">
         <v>0.2</v>
@@ -3774,8 +3779,15 @@
         <f t="shared" si="1"/>
         <v>0.27999999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>0.42</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="9">
         <v>0.35</v>
@@ -3803,8 +3815,12 @@
         <f t="shared" si="1"/>
         <v>0.11</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="9">
         <v>0.4</v>
@@ -3832,8 +3848,12 @@
         <f t="shared" si="1"/>
         <v>5.1000000000000004E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>0.24899999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="9">
         <v>0.5</v>
@@ -3861,8 +3881,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="9">
         <v>0.7</v>
@@ -3890,8 +3914,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="9">
         <v>0.9</v>
@@ -3919,8 +3947,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="9">
         <v>1.2</v>
@@ -3946,8 +3978,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="10">
         <v>2</v>
@@ -3973,8 +4009,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
@@ -4005,7 +4045,7 @@
         <v>0.248</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="9">
         <v>0.1</v>
@@ -4034,7 +4074,7 @@
         <v>0.22939999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="9">
         <v>0.2</v>
@@ -4063,7 +4103,7 @@
         <v>5.1000000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="9">
         <v>0.3</v>

</xml_diff>